<commit_message>
<Commit> Upload Excel File
</commit_message>
<xml_diff>
--- a/SIT-IT-Transcript.xlsx
+++ b/SIT-IT-Transcript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/purichsangprasert/Desktop/GethLearn/VeryFind_Transcript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A1BE95-F036-9B4E-92D6-D30107ABDA88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CA029E-9ADA-FD45-BECE-10D76B82F70A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="57130500060" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="98">
   <si>
     <t>semesterTitle</t>
   </si>
@@ -303,12 +303,6 @@
     <t>Mr.Purich Sangprasert</t>
   </si>
   <si>
-    <t>Mrs.Budsagorn Pakdeewan</t>
-  </si>
-  <si>
-    <t>Mrs.Mattana Thanuwong</t>
-  </si>
-  <si>
     <t>March 4,1998</t>
   </si>
   <si>
@@ -322,6 +316,15 @@
   </si>
   <si>
     <t>March 12, 1997</t>
+  </si>
+  <si>
+    <t>Ms.Mattana Thanuwong</t>
+  </si>
+  <si>
+    <t>Ms.Budsagorn Pakdeewan</t>
+  </si>
+  <si>
+    <t>June 4, 2020</t>
   </si>
 </sst>
 </file>
@@ -382,22 +385,75 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="130">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -408,93 +464,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -548,6 +521,63 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -565,76 +595,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -732,6 +696,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -829,6 +811,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -879,96 +882,96 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="KMUTT_Transcript_57130500060" displayName="KMUTT_Transcript_57130500060" ref="A1:P2" headerRowDxfId="129" dataDxfId="128">
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="studentID" totalsRowLabel="Total" dataDxfId="127" totalsRowDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="46" totalsRowDxfId="125"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="dob" dataDxfId="44" totalsRowDxfId="124"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="previousCert_Degree" dataDxfId="45" totalsRowDxfId="123"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="dateOfAdmission" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="dateOfGraduation" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="faculty" dataDxfId="10" totalsRowDxfId="122"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="fieldOfStudy" dataDxfId="121" totalsRowDxfId="120"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="major" dataDxfId="119" totalsRowDxfId="118"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="degreeConferred" dataDxfId="117" totalsRowDxfId="116"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="creditPrescribed" dataDxfId="115" totalsRowDxfId="114"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="creditsEarned" dataDxfId="113" totalsRowDxfId="112"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="totalGradGPA" dataDxfId="111" totalsRowDxfId="110"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="graduateHonors" dataDxfId="109" totalsRowDxfId="108"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="dateOfValidSeal" dataDxfId="107" totalsRowDxfId="106"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="registrar" totalsRowFunction="count" dataDxfId="105" totalsRowDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name" dataDxfId="125" totalsRowDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="dob" dataDxfId="123" totalsRowDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="previousCert_Degree" dataDxfId="121" totalsRowDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="dateOfAdmission" dataDxfId="119"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="dateOfGraduation" dataDxfId="118"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="faculty" dataDxfId="117" totalsRowDxfId="116"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="fieldOfStudy" dataDxfId="115" totalsRowDxfId="114"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="major" dataDxfId="113" totalsRowDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="degreeConferred" dataDxfId="111" totalsRowDxfId="110"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="creditPrescribed" dataDxfId="109" totalsRowDxfId="108"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="creditsEarned" dataDxfId="107" totalsRowDxfId="106"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="totalGradGPA" dataDxfId="105" totalsRowDxfId="104"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="graduateHonors" dataDxfId="103" totalsRowDxfId="102"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="dateOfValidSeal" dataDxfId="101" totalsRowDxfId="100"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="registrar" totalsRowFunction="count" dataDxfId="99" totalsRowDxfId="98"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{96854225-5795-EC48-B622-54AAF5BC541A}" name="KMUTT_Transcript_5713050006034" displayName="KMUTT_Transcript_5713050006034" ref="A1:P2" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{96854225-5795-EC48-B622-54AAF5BC541A}" name="KMUTT_Transcript_5713050006034" displayName="KMUTT_Transcript_5713050006034" ref="A1:P2" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{6396C84E-5CA0-B846-9151-CD120C3E4613}" name="studentID" totalsRowLabel="Total" dataDxfId="37" totalsRowDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{CEE03F1B-8603-C14F-B4C6-68168851C248}" name="name" dataDxfId="35" totalsRowDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{154F4134-D914-8D41-BA0B-DD2B1E15C929}" name="dob" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{2B098E13-CCA0-4948-8D5B-0763FD01B49A}" name="previousCert_Degree" dataDxfId="32" totalsRowDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{650AEA73-63B6-1D4F-8033-ABB7E4EE795B}" name="dateOfAdmission" dataDxfId="8" totalsRowDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{58629750-3B19-694B-A246-27FA3747AEA0}" name="dateOfGraduation" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{7ED2F313-BD7B-064A-8834-9DE91E06ABED}" name="faculty" dataDxfId="7" totalsRowDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{5CD7FCD0-523E-F149-A466-96BA4758846D}" name="fieldOfStudy" dataDxfId="28" totalsRowDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{E0CE8643-9242-D545-AE93-324B64632358}" name="major" dataDxfId="26" totalsRowDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{D0536623-E243-584C-9B86-723E6AC825C7}" name="degreeConferred" dataDxfId="24" totalsRowDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{1FBA5BC5-4996-E544-88BC-7655CFE84DD1}" name="creditPrescribed" dataDxfId="22" totalsRowDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{DB0025C7-C476-AC48-B7CD-C6E3BE28F659}" name="creditsEarned" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{AFD7CB4F-4510-474A-A0E2-FEA3BE3FFB6F}" name="totalGradGPA" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{F4DEE1EE-2D84-6948-BF0D-3E519FB9BE96}" name="graduateHonors" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{4DC25E56-0EF5-3E43-AFA1-0EA6260F086E}" name="dateOfValidSeal" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{A5DEA6DF-FCA1-174B-BEA4-A28744BE043A}" name="registrar" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{6396C84E-5CA0-B846-9151-CD120C3E4613}" name="studentID" totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{CEE03F1B-8603-C14F-B4C6-68168851C248}" name="name" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{154F4134-D914-8D41-BA0B-DD2B1E15C929}" name="dob" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{2B098E13-CCA0-4948-8D5B-0763FD01B49A}" name="previousCert_Degree" dataDxfId="90" totalsRowDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{650AEA73-63B6-1D4F-8033-ABB7E4EE795B}" name="dateOfAdmission" dataDxfId="88" totalsRowDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{58629750-3B19-694B-A246-27FA3747AEA0}" name="dateOfGraduation" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{7ED2F313-BD7B-064A-8834-9DE91E06ABED}" name="faculty" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="8" xr3:uid="{5CD7FCD0-523E-F149-A466-96BA4758846D}" name="fieldOfStudy" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="9" xr3:uid="{E0CE8643-9242-D545-AE93-324B64632358}" name="major" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="10" xr3:uid="{D0536623-E243-584C-9B86-723E6AC825C7}" name="degreeConferred" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="11" xr3:uid="{1FBA5BC5-4996-E544-88BC-7655CFE84DD1}" name="creditPrescribed" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="12" xr3:uid="{DB0025C7-C476-AC48-B7CD-C6E3BE28F659}" name="creditsEarned" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="13" xr3:uid="{AFD7CB4F-4510-474A-A0E2-FEA3BE3FFB6F}" name="totalGradGPA" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="14" xr3:uid="{F4DEE1EE-2D84-6948-BF0D-3E519FB9BE96}" name="graduateHonors" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="15" xr3:uid="{4DC25E56-0EF5-3E43-AFA1-0EA6260F086E}" name="dateOfValidSeal" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="16" xr3:uid="{A5DEA6DF-FCA1-174B-BEA4-A28744BE043A}" name="registrar" totalsRowFunction="count" dataDxfId="67" totalsRowDxfId="66"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79D55725-D763-E649-9658-74957C16105C}" name="KMUTT_Transcript_571305000603" displayName="KMUTT_Transcript_571305000603" ref="A1:P2" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79D55725-D763-E649-9658-74957C16105C}" name="KMUTT_Transcript_571305000603" displayName="KMUTT_Transcript_571305000603" ref="A1:P2" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{8A21E65E-A648-AF4F-ABEA-5A9824EA0F6F}" name="studentID" totalsRowLabel="Total" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="2" xr3:uid="{E12E4376-D1D8-9B41-9FEC-1E15A494FA7D}" name="name" dataDxfId="49" totalsRowDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{45150663-D20F-3246-AC8F-83F6BD9C8798}" name="dob" dataDxfId="47" totalsRowDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{2455CD3C-3084-A741-82DC-331A13265348}" name="previousCert_Degree" dataDxfId="48" totalsRowDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{9BD65584-7AE4-D042-81F8-54976979CF81}" name="dateOfAdmission" dataDxfId="5" totalsRowDxfId="96"/>
-    <tableColumn id="6" xr3:uid="{87AEAB75-A71E-114B-A9F1-9B15862E6CC9}" name="dateOfGraduation" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{781BD1A0-4ECE-2247-A5FA-96134F17B17F}" name="faculty" dataDxfId="4" totalsRowDxfId="95"/>
-    <tableColumn id="8" xr3:uid="{9B8CB910-6ADE-674D-A515-E4AA3B83F301}" name="fieldOfStudy" dataDxfId="94" totalsRowDxfId="93"/>
-    <tableColumn id="9" xr3:uid="{F5969211-C464-FC4D-A108-5B0664933525}" name="major" dataDxfId="92" totalsRowDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{060CA6A3-8634-BF4C-99CA-F5C3CC1ED649}" name="degreeConferred" dataDxfId="90" totalsRowDxfId="89"/>
-    <tableColumn id="11" xr3:uid="{8AD00EA8-AFC3-FA4E-87FD-EF6A5EE21401}" name="creditPrescribed" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="12" xr3:uid="{A120D8AE-8A1E-B645-98ED-AA2544409F3D}" name="creditsEarned" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="13" xr3:uid="{4D4888BD-EA84-3B4A-852F-47B1AD775715}" name="totalGradGPA" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="14" xr3:uid="{9D9959DF-E5D6-6740-9E26-39E416AE78A6}" name="graduateHonors" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="15" xr3:uid="{A5FDCC8E-FB31-6943-B743-B91C21B4B56D}" name="dateOfValidSeal" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="16" xr3:uid="{E3D2C7C4-D6D1-084F-9031-2DF7B6F7ECAE}" name="registrar" totalsRowFunction="count" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{8A21E65E-A648-AF4F-ABEA-5A9824EA0F6F}" name="studentID" totalsRowLabel="Total" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{E12E4376-D1D8-9B41-9FEC-1E15A494FA7D}" name="name" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{45150663-D20F-3246-AC8F-83F6BD9C8798}" name="dob" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{2455CD3C-3084-A741-82DC-331A13265348}" name="previousCert_Degree" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{9BD65584-7AE4-D042-81F8-54976979CF81}" name="dateOfAdmission" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{87AEAB75-A71E-114B-A9F1-9B15862E6CC9}" name="dateOfGraduation" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{781BD1A0-4ECE-2247-A5FA-96134F17B17F}" name="faculty" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{9B8CB910-6ADE-674D-A515-E4AA3B83F301}" name="fieldOfStudy" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{F5969211-C464-FC4D-A108-5B0664933525}" name="major" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{060CA6A3-8634-BF4C-99CA-F5C3CC1ED649}" name="degreeConferred" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{8AD00EA8-AFC3-FA4E-87FD-EF6A5EE21401}" name="creditPrescribed" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{A120D8AE-8A1E-B645-98ED-AA2544409F3D}" name="creditsEarned" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{4D4888BD-EA84-3B4A-852F-47B1AD775715}" name="totalGradGPA" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{9D9959DF-E5D6-6740-9E26-39E416AE78A6}" name="graduateHonors" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="15" xr3:uid="{A5FDCC8E-FB31-6943-B743-B91C21B4B56D}" name="dateOfValidSeal" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="16" xr3:uid="{E3D2C7C4-D6D1-084F-9031-2DF7B6F7ECAE}" name="registrar" totalsRowFunction="count" dataDxfId="34" totalsRowDxfId="33"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F59993DF-D6AB-5F49-94AC-4C40BDC31A97}" name="KMUTT_Transcript_5713050006035" displayName="KMUTT_Transcript_5713050006035" ref="A1:P2" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F59993DF-D6AB-5F49-94AC-4C40BDC31A97}" name="KMUTT_Transcript_5713050006035" displayName="KMUTT_Transcript_5713050006035" ref="A1:P2" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{1509A60D-9089-5247-978C-6A4103B9C32B}" name="studentID" totalsRowLabel="Total" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{94E03D94-CA36-8446-9BA4-78B3410003FC}" name="name" dataDxfId="43" totalsRowDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{B769A1E8-7673-A84F-8E8E-7D052F596944}" name="dob" dataDxfId="42" totalsRowDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{7CE4B67F-7F4E-6143-9210-B15A6B792389}" name="previousCert_Degree" dataDxfId="41" totalsRowDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{492D7C75-22A1-AE40-A6C1-799AD5E1008D}" name="dateOfAdmission" dataDxfId="2" totalsRowDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{1C0632CA-4DEE-4946-8C5E-2F30CD4C3ABF}" name="dateOfGraduation" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{76A9D9B2-BA43-B34D-8503-780F06A6711E}" name="faculty" dataDxfId="1" totalsRowDxfId="68"/>
-    <tableColumn id="8" xr3:uid="{ED8DEE61-2DF7-6E46-8955-7E05068BF784}" name="fieldOfStudy" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{D8A90C32-76A2-6A4D-A5BC-510C0C482283}" name="major" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{A7252744-7D19-1341-A8F8-77A8568C1AA1}" name="degreeConferred" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{69B88F12-0DA3-1A4A-B320-600429250028}" name="creditPrescribed" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{77978312-48C9-8945-B96D-353677C20B1C}" name="creditsEarned" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{3B385A57-993D-104A-9F02-7636156099AF}" name="totalGradGPA" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{0FC66D71-6218-0746-A1E9-9185A55B2779}" name="graduateHonors" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{43C481DC-616D-1D43-9FEB-4A2E08D2CDD8}" name="dateOfValidSeal" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="16" xr3:uid="{B14B94D2-F6F1-4D42-A011-687852A5D491}" name="registrar" totalsRowFunction="count" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{1509A60D-9089-5247-978C-6A4103B9C32B}" name="studentID" totalsRowLabel="Total" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{94E03D94-CA36-8446-9BA4-78B3410003FC}" name="name" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{B769A1E8-7673-A84F-8E8E-7D052F596944}" name="dob" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{7CE4B67F-7F4E-6143-9210-B15A6B792389}" name="previousCert_Degree" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{492D7C75-22A1-AE40-A6C1-799AD5E1008D}" name="dateOfAdmission" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{1C0632CA-4DEE-4946-8C5E-2F30CD4C3ABF}" name="dateOfGraduation" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{76A9D9B2-BA43-B34D-8503-780F06A6711E}" name="faculty" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{ED8DEE61-2DF7-6E46-8955-7E05068BF784}" name="fieldOfStudy" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{D8A90C32-76A2-6A4D-A5BC-510C0C482283}" name="major" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{A7252744-7D19-1341-A8F8-77A8568C1AA1}" name="degreeConferred" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{69B88F12-0DA3-1A4A-B320-600429250028}" name="creditPrescribed" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{77978312-48C9-8945-B96D-353677C20B1C}" name="creditsEarned" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3B385A57-993D-104A-9F02-7636156099AF}" name="totalGradGPA" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{0FC66D71-6218-0746-A1E9-9185A55B2779}" name="graduateHonors" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{43C481DC-616D-1D43-9FEB-4A2E08D2CDD8}" name="dateOfValidSeal" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{B14B94D2-F6F1-4D42-A011-687852A5D491}" name="registrar" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1473,17 +1476,17 @@
       <c r="B2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>75</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>94</v>
+      <c r="E2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>77</v>
@@ -1513,16 +1516,16 @@
       <c r="P2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="7">
         <v>16</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="7">
         <v>3.5</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="7">
         <v>3.5</v>
       </c>
       <c r="U2" t="s">
@@ -1536,10 +1539,10 @@
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
       <c r="U3" t="s">
         <v>4</v>
       </c>
@@ -1552,10 +1555,10 @@
     </row>
     <row r="4" spans="1:23">
       <c r="E4" s="3"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
       <c r="U4" t="s">
         <v>5</v>
       </c>
@@ -1567,10 +1570,10 @@
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
       <c r="U5" t="s">
         <v>7</v>
       </c>
@@ -1582,10 +1585,10 @@
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
       <c r="U6" t="s">
         <v>8</v>
       </c>
@@ -1597,10 +1600,10 @@
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
       <c r="U7" t="s">
         <v>10</v>
       </c>
@@ -1612,16 +1615,16 @@
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="7">
         <v>18</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="7">
         <v>3.58</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="7">
         <v>3.35</v>
       </c>
       <c r="U8" t="s">
@@ -1635,10 +1638,10 @@
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
       <c r="U9" t="s">
         <v>14</v>
       </c>
@@ -1650,10 +1653,10 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
       <c r="U10" t="s">
         <v>15</v>
       </c>
@@ -1665,10 +1668,10 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
       <c r="U11" t="s">
         <v>16</v>
       </c>
@@ -1680,10 +1683,10 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
       <c r="U12" t="s">
         <v>17</v>
       </c>
@@ -1695,10 +1698,10 @@
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
       <c r="U13" t="s">
         <v>18</v>
       </c>
@@ -1710,16 +1713,16 @@
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="Q14" s="5" t="s">
+      <c r="Q14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="7">
         <v>18</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="7">
         <v>3.33</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="7">
         <v>3.35</v>
       </c>
       <c r="U14" t="s">
@@ -1733,10 +1736,10 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
       <c r="U15" t="s">
         <v>22</v>
       </c>
@@ -1748,10 +1751,10 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
       <c r="U16" t="s">
         <v>23</v>
       </c>
@@ -1763,10 +1766,10 @@
       </c>
     </row>
     <row r="17" spans="17:23">
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
       <c r="U17" t="s">
         <v>24</v>
       </c>
@@ -1778,10 +1781,10 @@
       </c>
     </row>
     <row r="18" spans="17:23">
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
       <c r="U18" t="s">
         <v>25</v>
       </c>
@@ -1793,10 +1796,10 @@
       </c>
     </row>
     <row r="19" spans="17:23">
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
       <c r="U19" t="s">
         <v>26</v>
       </c>
@@ -1808,16 +1811,16 @@
       </c>
     </row>
     <row r="20" spans="17:23">
-      <c r="Q20" s="5" t="s">
+      <c r="Q20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="7">
         <v>18</v>
       </c>
-      <c r="S20" s="5">
+      <c r="S20" s="7">
         <v>3.33</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="7">
         <v>3.35</v>
       </c>
       <c r="U20" t="s">
@@ -1831,10 +1834,10 @@
       </c>
     </row>
     <row r="21" spans="17:23">
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
       <c r="U21" t="s">
         <v>29</v>
       </c>
@@ -1846,10 +1849,10 @@
       </c>
     </row>
     <row r="22" spans="17:23">
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
       <c r="U22" t="s">
         <v>30</v>
       </c>
@@ -1861,10 +1864,10 @@
       </c>
     </row>
     <row r="23" spans="17:23">
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
       <c r="U23" t="s">
         <v>31</v>
       </c>
@@ -1876,10 +1879,10 @@
       </c>
     </row>
     <row r="24" spans="17:23">
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
       <c r="U24" t="s">
         <v>32</v>
       </c>
@@ -1891,10 +1894,10 @@
       </c>
     </row>
     <row r="25" spans="17:23">
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
       <c r="U25" t="s">
         <v>33</v>
       </c>
@@ -1906,16 +1909,16 @@
       </c>
     </row>
     <row r="26" spans="17:23">
-      <c r="Q26" s="5" t="s">
+      <c r="Q26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="7">
         <v>19</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="7">
         <v>3.42</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="7">
         <v>3.36</v>
       </c>
       <c r="U26" t="s">
@@ -1929,10 +1932,10 @@
       </c>
     </row>
     <row r="27" spans="17:23">
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
       <c r="U27" t="s">
         <v>36</v>
       </c>
@@ -1944,10 +1947,10 @@
       </c>
     </row>
     <row r="28" spans="17:23">
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
       <c r="U28" t="s">
         <v>37</v>
       </c>
@@ -1959,10 +1962,10 @@
       </c>
     </row>
     <row r="29" spans="17:23">
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
       <c r="U29" t="s">
         <v>38</v>
       </c>
@@ -1974,10 +1977,10 @@
       </c>
     </row>
     <row r="30" spans="17:23">
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
       <c r="U30" t="s">
         <v>39</v>
       </c>
@@ -1989,10 +1992,10 @@
       </c>
     </row>
     <row r="31" spans="17:23">
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
       <c r="U31" t="s">
         <v>40</v>
       </c>
@@ -2004,10 +2007,10 @@
       </c>
     </row>
     <row r="32" spans="17:23">
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
       <c r="U32" t="s">
         <v>41</v>
       </c>
@@ -2019,16 +2022,16 @@
       </c>
     </row>
     <row r="33" spans="17:23">
-      <c r="Q33" s="5" t="s">
+      <c r="Q33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="R33" s="5">
+      <c r="R33" s="7">
         <v>14</v>
       </c>
-      <c r="S33" s="5">
+      <c r="S33" s="7">
         <v>2.96</v>
       </c>
-      <c r="T33" s="5">
+      <c r="T33" s="7">
         <v>3.31</v>
       </c>
       <c r="U33" t="s">
@@ -2042,10 +2045,10 @@
       </c>
     </row>
     <row r="34" spans="17:23">
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
       <c r="U34" t="s">
         <v>44</v>
       </c>
@@ -2057,10 +2060,10 @@
       </c>
     </row>
     <row r="35" spans="17:23">
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
       <c r="U35" t="s">
         <v>45</v>
       </c>
@@ -2072,10 +2075,10 @@
       </c>
     </row>
     <row r="36" spans="17:23">
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
       <c r="U36" t="s">
         <v>46</v>
       </c>
@@ -2087,10 +2090,10 @@
       </c>
     </row>
     <row r="37" spans="17:23">
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
       <c r="U37" t="s">
         <v>47</v>
       </c>
@@ -2102,16 +2105,16 @@
       </c>
     </row>
     <row r="38" spans="17:23">
-      <c r="Q38" s="5" t="s">
+      <c r="Q38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="R38" s="5">
+      <c r="R38" s="7">
         <v>17</v>
       </c>
-      <c r="S38" s="5">
+      <c r="S38" s="7">
         <v>3.47</v>
       </c>
-      <c r="T38" s="5">
+      <c r="T38" s="7">
         <v>3.33</v>
       </c>
       <c r="U38" t="s">
@@ -2125,10 +2128,10 @@
       </c>
     </row>
     <row r="39" spans="17:23">
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
       <c r="U39" t="s">
         <v>50</v>
       </c>
@@ -2140,10 +2143,10 @@
       </c>
     </row>
     <row r="40" spans="17:23">
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
       <c r="U40" t="s">
         <v>51</v>
       </c>
@@ -2155,10 +2158,10 @@
       </c>
     </row>
     <row r="41" spans="17:23">
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
       <c r="U41" t="s">
         <v>52</v>
       </c>
@@ -2170,10 +2173,10 @@
       </c>
     </row>
     <row r="42" spans="17:23">
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
       <c r="U42" t="s">
         <v>47</v>
       </c>
@@ -2185,10 +2188,10 @@
       </c>
     </row>
     <row r="43" spans="17:23">
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
       <c r="U43" t="s">
         <v>53</v>
       </c>
@@ -2200,16 +2203,16 @@
       </c>
     </row>
     <row r="44" spans="17:23">
-      <c r="Q44" s="5" t="s">
+      <c r="Q44" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R44" s="5">
-        <v>9</v>
-      </c>
-      <c r="S44" s="5">
+      <c r="R44" s="7">
+        <v>9</v>
+      </c>
+      <c r="S44" s="7">
         <v>3.5</v>
       </c>
-      <c r="T44" s="5">
+      <c r="T44" s="7">
         <v>3.34</v>
       </c>
       <c r="U44" t="s">
@@ -2223,10 +2226,10 @@
       </c>
     </row>
     <row r="45" spans="17:23">
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
       <c r="U45" t="s">
         <v>56</v>
       </c>
@@ -2238,10 +2241,10 @@
       </c>
     </row>
     <row r="46" spans="17:23">
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
       <c r="U46" t="s">
         <v>57</v>
       </c>
@@ -2417,19 +2420,19 @@
         <v>59130500045</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>93</v>
+      <c r="E2" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>77</v>
@@ -2459,16 +2462,16 @@
       <c r="P2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="7">
         <v>16</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="7">
         <v>3.5</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="7">
         <v>3.5</v>
       </c>
       <c r="U2" t="s">
@@ -2482,10 +2485,10 @@
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
       <c r="U3" t="s">
         <v>4</v>
       </c>
@@ -2497,10 +2500,10 @@
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
       <c r="U4" t="s">
         <v>5</v>
       </c>
@@ -2512,10 +2515,10 @@
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
       <c r="U5" t="s">
         <v>7</v>
       </c>
@@ -2527,10 +2530,10 @@
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
       <c r="U6" t="s">
         <v>8</v>
       </c>
@@ -2542,10 +2545,10 @@
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
       <c r="U7" t="s">
         <v>10</v>
       </c>
@@ -2557,16 +2560,16 @@
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="7">
         <v>18</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="7">
         <v>3.58</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="7">
         <v>3.35</v>
       </c>
       <c r="U8" t="s">
@@ -2580,10 +2583,10 @@
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
       <c r="U9" t="s">
         <v>14</v>
       </c>
@@ -2595,10 +2598,10 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
       <c r="U10" t="s">
         <v>15</v>
       </c>
@@ -2610,10 +2613,10 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
       <c r="U11" t="s">
         <v>16</v>
       </c>
@@ -2625,10 +2628,10 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
       <c r="U12" t="s">
         <v>17</v>
       </c>
@@ -2640,10 +2643,10 @@
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
       <c r="U13" t="s">
         <v>18</v>
       </c>
@@ -2655,16 +2658,16 @@
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="Q14" s="5" t="s">
+      <c r="Q14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="7">
         <v>18</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="7">
         <v>3.33</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="7">
         <v>3.35</v>
       </c>
       <c r="U14" t="s">
@@ -2678,10 +2681,10 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
       <c r="U15" t="s">
         <v>22</v>
       </c>
@@ -2693,10 +2696,10 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
       <c r="U16" t="s">
         <v>23</v>
       </c>
@@ -2708,10 +2711,10 @@
       </c>
     </row>
     <row r="17" spans="17:23">
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
       <c r="U17" t="s">
         <v>24</v>
       </c>
@@ -2723,10 +2726,10 @@
       </c>
     </row>
     <row r="18" spans="17:23">
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
       <c r="U18" t="s">
         <v>25</v>
       </c>
@@ -2738,10 +2741,10 @@
       </c>
     </row>
     <row r="19" spans="17:23">
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
       <c r="U19" t="s">
         <v>26</v>
       </c>
@@ -2753,16 +2756,16 @@
       </c>
     </row>
     <row r="20" spans="17:23">
-      <c r="Q20" s="5" t="s">
+      <c r="Q20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="7">
         <v>18</v>
       </c>
-      <c r="S20" s="5">
+      <c r="S20" s="7">
         <v>3.33</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="7">
         <v>3.35</v>
       </c>
       <c r="U20" t="s">
@@ -2776,10 +2779,10 @@
       </c>
     </row>
     <row r="21" spans="17:23">
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
       <c r="U21" t="s">
         <v>29</v>
       </c>
@@ -2791,10 +2794,10 @@
       </c>
     </row>
     <row r="22" spans="17:23">
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
       <c r="U22" t="s">
         <v>30</v>
       </c>
@@ -2806,10 +2809,10 @@
       </c>
     </row>
     <row r="23" spans="17:23">
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
       <c r="U23" t="s">
         <v>31</v>
       </c>
@@ -2821,10 +2824,10 @@
       </c>
     </row>
     <row r="24" spans="17:23">
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
       <c r="U24" t="s">
         <v>32</v>
       </c>
@@ -2836,10 +2839,10 @@
       </c>
     </row>
     <row r="25" spans="17:23">
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
       <c r="U25" t="s">
         <v>33</v>
       </c>
@@ -2851,16 +2854,16 @@
       </c>
     </row>
     <row r="26" spans="17:23">
-      <c r="Q26" s="5" t="s">
+      <c r="Q26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="7">
         <v>19</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="7">
         <v>3.42</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="7">
         <v>3.36</v>
       </c>
       <c r="U26" t="s">
@@ -2874,10 +2877,10 @@
       </c>
     </row>
     <row r="27" spans="17:23">
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
       <c r="U27" t="s">
         <v>36</v>
       </c>
@@ -2889,10 +2892,10 @@
       </c>
     </row>
     <row r="28" spans="17:23">
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
       <c r="U28" t="s">
         <v>37</v>
       </c>
@@ -2904,10 +2907,10 @@
       </c>
     </row>
     <row r="29" spans="17:23">
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
       <c r="U29" t="s">
         <v>38</v>
       </c>
@@ -2919,10 +2922,10 @@
       </c>
     </row>
     <row r="30" spans="17:23">
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
       <c r="U30" t="s">
         <v>39</v>
       </c>
@@ -2934,10 +2937,10 @@
       </c>
     </row>
     <row r="31" spans="17:23">
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
       <c r="U31" t="s">
         <v>40</v>
       </c>
@@ -2949,10 +2952,10 @@
       </c>
     </row>
     <row r="32" spans="17:23">
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
       <c r="U32" t="s">
         <v>41</v>
       </c>
@@ -2964,16 +2967,16 @@
       </c>
     </row>
     <row r="33" spans="17:23">
-      <c r="Q33" s="5" t="s">
+      <c r="Q33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="R33" s="5">
+      <c r="R33" s="7">
         <v>14</v>
       </c>
-      <c r="S33" s="5">
+      <c r="S33" s="7">
         <v>2.96</v>
       </c>
-      <c r="T33" s="5">
+      <c r="T33" s="7">
         <v>3.31</v>
       </c>
       <c r="U33" t="s">
@@ -2987,10 +2990,10 @@
       </c>
     </row>
     <row r="34" spans="17:23">
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
       <c r="U34" t="s">
         <v>44</v>
       </c>
@@ -3002,10 +3005,10 @@
       </c>
     </row>
     <row r="35" spans="17:23">
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
       <c r="U35" t="s">
         <v>45</v>
       </c>
@@ -3017,10 +3020,10 @@
       </c>
     </row>
     <row r="36" spans="17:23">
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
       <c r="U36" t="s">
         <v>46</v>
       </c>
@@ -3032,10 +3035,10 @@
       </c>
     </row>
     <row r="37" spans="17:23">
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
       <c r="U37" t="s">
         <v>47</v>
       </c>
@@ -3047,16 +3050,16 @@
       </c>
     </row>
     <row r="38" spans="17:23">
-      <c r="Q38" s="5" t="s">
+      <c r="Q38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="R38" s="5">
+      <c r="R38" s="7">
         <v>17</v>
       </c>
-      <c r="S38" s="5">
+      <c r="S38" s="7">
         <v>3.47</v>
       </c>
-      <c r="T38" s="5">
+      <c r="T38" s="7">
         <v>3.33</v>
       </c>
       <c r="U38" t="s">
@@ -3070,10 +3073,10 @@
       </c>
     </row>
     <row r="39" spans="17:23">
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
       <c r="U39" t="s">
         <v>50</v>
       </c>
@@ -3085,10 +3088,10 @@
       </c>
     </row>
     <row r="40" spans="17:23">
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
       <c r="U40" t="s">
         <v>51</v>
       </c>
@@ -3100,10 +3103,10 @@
       </c>
     </row>
     <row r="41" spans="17:23">
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
       <c r="U41" t="s">
         <v>52</v>
       </c>
@@ -3115,10 +3118,10 @@
       </c>
     </row>
     <row r="42" spans="17:23">
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
       <c r="U42" t="s">
         <v>47</v>
       </c>
@@ -3130,10 +3133,10 @@
       </c>
     </row>
     <row r="43" spans="17:23">
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
       <c r="U43" t="s">
         <v>53</v>
       </c>
@@ -3145,16 +3148,16 @@
       </c>
     </row>
     <row r="44" spans="17:23">
-      <c r="Q44" s="5" t="s">
+      <c r="Q44" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R44" s="5">
-        <v>9</v>
-      </c>
-      <c r="S44" s="5">
+      <c r="R44" s="7">
+        <v>9</v>
+      </c>
+      <c r="S44" s="7">
         <v>3.5</v>
       </c>
-      <c r="T44" s="5">
+      <c r="T44" s="7">
         <v>3.34</v>
       </c>
       <c r="U44" t="s">
@@ -3168,10 +3171,10 @@
       </c>
     </row>
     <row r="45" spans="17:23">
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
       <c r="U45" t="s">
         <v>56</v>
       </c>
@@ -3183,10 +3186,10 @@
       </c>
     </row>
     <row r="46" spans="17:23">
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
       <c r="U46" t="s">
         <v>57</v>
       </c>
@@ -3249,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA81AC1C-250F-2548-9534-F412F93EB1B7}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -3364,17 +3367,17 @@
       <c r="B2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>92</v>
+      <c r="C2" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>93</v>
+      <c r="E2" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>77</v>
@@ -3404,16 +3407,16 @@
       <c r="P2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="7">
         <v>16</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="7">
         <v>3.5</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="7">
         <v>3.5</v>
       </c>
       <c r="U2" t="s">
@@ -3427,10 +3430,10 @@
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
       <c r="U3" t="s">
         <v>4</v>
       </c>
@@ -3442,10 +3445,10 @@
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
       <c r="U4" t="s">
         <v>5</v>
       </c>
@@ -3457,10 +3460,10 @@
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
       <c r="U5" t="s">
         <v>7</v>
       </c>
@@ -3472,10 +3475,10 @@
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
       <c r="U6" t="s">
         <v>8</v>
       </c>
@@ -3487,10 +3490,10 @@
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
       <c r="U7" t="s">
         <v>10</v>
       </c>
@@ -3502,16 +3505,16 @@
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="7">
         <v>18</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="7">
         <v>3.58</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="7">
         <v>3.35</v>
       </c>
       <c r="U8" t="s">
@@ -3525,10 +3528,10 @@
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
       <c r="U9" t="s">
         <v>14</v>
       </c>
@@ -3540,10 +3543,10 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
       <c r="U10" t="s">
         <v>15</v>
       </c>
@@ -3555,10 +3558,10 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
       <c r="U11" t="s">
         <v>16</v>
       </c>
@@ -3570,10 +3573,10 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
       <c r="U12" t="s">
         <v>17</v>
       </c>
@@ -3585,10 +3588,10 @@
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
       <c r="U13" t="s">
         <v>18</v>
       </c>
@@ -3600,16 +3603,16 @@
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="Q14" s="5" t="s">
+      <c r="Q14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="7">
         <v>18</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="7">
         <v>3.33</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="7">
         <v>3.35</v>
       </c>
       <c r="U14" t="s">
@@ -3623,10 +3626,10 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
       <c r="U15" t="s">
         <v>22</v>
       </c>
@@ -3638,10 +3641,10 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
       <c r="U16" t="s">
         <v>23</v>
       </c>
@@ -3653,10 +3656,10 @@
       </c>
     </row>
     <row r="17" spans="17:23">
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
       <c r="U17" t="s">
         <v>24</v>
       </c>
@@ -3668,10 +3671,10 @@
       </c>
     </row>
     <row r="18" spans="17:23">
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
       <c r="U18" t="s">
         <v>25</v>
       </c>
@@ -3683,10 +3686,10 @@
       </c>
     </row>
     <row r="19" spans="17:23">
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
       <c r="U19" t="s">
         <v>26</v>
       </c>
@@ -3698,16 +3701,16 @@
       </c>
     </row>
     <row r="20" spans="17:23">
-      <c r="Q20" s="5" t="s">
+      <c r="Q20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="7">
         <v>18</v>
       </c>
-      <c r="S20" s="5">
+      <c r="S20" s="7">
         <v>3.33</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="7">
         <v>3.35</v>
       </c>
       <c r="U20" t="s">
@@ -3721,10 +3724,10 @@
       </c>
     </row>
     <row r="21" spans="17:23">
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
       <c r="U21" t="s">
         <v>29</v>
       </c>
@@ -3736,10 +3739,10 @@
       </c>
     </row>
     <row r="22" spans="17:23">
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
       <c r="U22" t="s">
         <v>30</v>
       </c>
@@ -3751,10 +3754,10 @@
       </c>
     </row>
     <row r="23" spans="17:23">
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
       <c r="U23" t="s">
         <v>31</v>
       </c>
@@ -3766,10 +3769,10 @@
       </c>
     </row>
     <row r="24" spans="17:23">
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
       <c r="U24" t="s">
         <v>32</v>
       </c>
@@ -3781,10 +3784,10 @@
       </c>
     </row>
     <row r="25" spans="17:23">
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
       <c r="U25" t="s">
         <v>33</v>
       </c>
@@ -3796,16 +3799,16 @@
       </c>
     </row>
     <row r="26" spans="17:23">
-      <c r="Q26" s="5" t="s">
+      <c r="Q26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="7">
         <v>19</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="7">
         <v>3.42</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="7">
         <v>3.36</v>
       </c>
       <c r="U26" t="s">
@@ -3819,10 +3822,10 @@
       </c>
     </row>
     <row r="27" spans="17:23">
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
       <c r="U27" t="s">
         <v>36</v>
       </c>
@@ -3834,10 +3837,10 @@
       </c>
     </row>
     <row r="28" spans="17:23">
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
       <c r="U28" t="s">
         <v>37</v>
       </c>
@@ -3849,10 +3852,10 @@
       </c>
     </row>
     <row r="29" spans="17:23">
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
       <c r="U29" t="s">
         <v>38</v>
       </c>
@@ -3864,10 +3867,10 @@
       </c>
     </row>
     <row r="30" spans="17:23">
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
       <c r="U30" t="s">
         <v>39</v>
       </c>
@@ -3879,10 +3882,10 @@
       </c>
     </row>
     <row r="31" spans="17:23">
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
       <c r="U31" t="s">
         <v>40</v>
       </c>
@@ -3894,10 +3897,10 @@
       </c>
     </row>
     <row r="32" spans="17:23">
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
       <c r="U32" t="s">
         <v>41</v>
       </c>
@@ -3909,16 +3912,16 @@
       </c>
     </row>
     <row r="33" spans="17:23">
-      <c r="Q33" s="5" t="s">
+      <c r="Q33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="R33" s="5">
+      <c r="R33" s="7">
         <v>14</v>
       </c>
-      <c r="S33" s="5">
+      <c r="S33" s="7">
         <v>2.96</v>
       </c>
-      <c r="T33" s="5">
+      <c r="T33" s="7">
         <v>3.31</v>
       </c>
       <c r="U33" t="s">
@@ -3932,10 +3935,10 @@
       </c>
     </row>
     <row r="34" spans="17:23">
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
       <c r="U34" t="s">
         <v>44</v>
       </c>
@@ -3947,10 +3950,10 @@
       </c>
     </row>
     <row r="35" spans="17:23">
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
       <c r="U35" t="s">
         <v>45</v>
       </c>
@@ -3962,10 +3965,10 @@
       </c>
     </row>
     <row r="36" spans="17:23">
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
       <c r="U36" t="s">
         <v>46</v>
       </c>
@@ -3977,10 +3980,10 @@
       </c>
     </row>
     <row r="37" spans="17:23">
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
       <c r="U37" t="s">
         <v>47</v>
       </c>
@@ -3992,16 +3995,16 @@
       </c>
     </row>
     <row r="38" spans="17:23">
-      <c r="Q38" s="5" t="s">
+      <c r="Q38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="R38" s="5">
+      <c r="R38" s="7">
         <v>17</v>
       </c>
-      <c r="S38" s="5">
+      <c r="S38" s="7">
         <v>3.47</v>
       </c>
-      <c r="T38" s="5">
+      <c r="T38" s="7">
         <v>3.33</v>
       </c>
       <c r="U38" t="s">
@@ -4015,10 +4018,10 @@
       </c>
     </row>
     <row r="39" spans="17:23">
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
       <c r="U39" t="s">
         <v>50</v>
       </c>
@@ -4030,10 +4033,10 @@
       </c>
     </row>
     <row r="40" spans="17:23">
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
       <c r="U40" t="s">
         <v>51</v>
       </c>
@@ -4045,10 +4048,10 @@
       </c>
     </row>
     <row r="41" spans="17:23">
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
       <c r="U41" t="s">
         <v>52</v>
       </c>
@@ -4060,10 +4063,10 @@
       </c>
     </row>
     <row r="42" spans="17:23">
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
       <c r="U42" t="s">
         <v>47</v>
       </c>
@@ -4075,10 +4078,10 @@
       </c>
     </row>
     <row r="43" spans="17:23">
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
       <c r="U43" t="s">
         <v>53</v>
       </c>
@@ -4090,16 +4093,16 @@
       </c>
     </row>
     <row r="44" spans="17:23">
-      <c r="Q44" s="5" t="s">
+      <c r="Q44" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R44" s="5">
-        <v>9</v>
-      </c>
-      <c r="S44" s="5">
+      <c r="R44" s="7">
+        <v>9</v>
+      </c>
+      <c r="S44" s="7">
         <v>3.5</v>
       </c>
-      <c r="T44" s="5">
+      <c r="T44" s="7">
         <v>3.34</v>
       </c>
       <c r="U44" t="s">
@@ -4113,10 +4116,10 @@
       </c>
     </row>
     <row r="45" spans="17:23">
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
       <c r="U45" t="s">
         <v>56</v>
       </c>
@@ -4128,10 +4131,10 @@
       </c>
     </row>
     <row r="46" spans="17:23">
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
       <c r="U46" t="s">
         <v>57</v>
       </c>
@@ -4194,8 +4197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4613129-E19C-AC4B-8BBB-030EBED8D8B0}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4307,19 +4310,19 @@
         <v>59130500072</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>93</v>
+      <c r="E2" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>77</v>
@@ -4349,16 +4352,16 @@
       <c r="P2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="7">
         <v>16</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="7">
         <v>3.5</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="7">
         <v>3.5</v>
       </c>
       <c r="U2" t="s">
@@ -4372,10 +4375,10 @@
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
       <c r="U3" t="s">
         <v>4</v>
       </c>
@@ -4387,10 +4390,10 @@
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
       <c r="U4" t="s">
         <v>5</v>
       </c>
@@ -4402,10 +4405,10 @@
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
       <c r="U5" t="s">
         <v>7</v>
       </c>
@@ -4417,10 +4420,10 @@
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
       <c r="U6" t="s">
         <v>8</v>
       </c>
@@ -4432,10 +4435,10 @@
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
       <c r="U7" t="s">
         <v>10</v>
       </c>
@@ -4447,16 +4450,16 @@
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="7">
         <v>18</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="7">
         <v>3.58</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="7">
         <v>3.35</v>
       </c>
       <c r="U8" t="s">
@@ -4470,10 +4473,10 @@
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
       <c r="U9" t="s">
         <v>14</v>
       </c>
@@ -4485,10 +4488,10 @@
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
       <c r="U10" t="s">
         <v>15</v>
       </c>
@@ -4500,10 +4503,10 @@
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
       <c r="U11" t="s">
         <v>16</v>
       </c>
@@ -4515,10 +4518,10 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
       <c r="U12" t="s">
         <v>17</v>
       </c>
@@ -4530,10 +4533,10 @@
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
       <c r="U13" t="s">
         <v>18</v>
       </c>
@@ -4545,16 +4548,16 @@
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="Q14" s="5" t="s">
+      <c r="Q14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="7">
         <v>18</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="7">
         <v>3.33</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="7">
         <v>3.35</v>
       </c>
       <c r="U14" t="s">
@@ -4568,10 +4571,10 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
       <c r="U15" t="s">
         <v>22</v>
       </c>
@@ -4583,10 +4586,10 @@
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
       <c r="U16" t="s">
         <v>23</v>
       </c>
@@ -4598,10 +4601,10 @@
       </c>
     </row>
     <row r="17" spans="17:23">
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
       <c r="U17" t="s">
         <v>24</v>
       </c>
@@ -4613,10 +4616,10 @@
       </c>
     </row>
     <row r="18" spans="17:23">
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
       <c r="U18" t="s">
         <v>25</v>
       </c>
@@ -4628,10 +4631,10 @@
       </c>
     </row>
     <row r="19" spans="17:23">
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
       <c r="U19" t="s">
         <v>26</v>
       </c>
@@ -4643,16 +4646,16 @@
       </c>
     </row>
     <row r="20" spans="17:23">
-      <c r="Q20" s="5" t="s">
+      <c r="Q20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="7">
         <v>18</v>
       </c>
-      <c r="S20" s="5">
+      <c r="S20" s="7">
         <v>3.33</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="7">
         <v>3.35</v>
       </c>
       <c r="U20" t="s">
@@ -4666,10 +4669,10 @@
       </c>
     </row>
     <row r="21" spans="17:23">
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
       <c r="U21" t="s">
         <v>29</v>
       </c>
@@ -4681,10 +4684,10 @@
       </c>
     </row>
     <row r="22" spans="17:23">
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
       <c r="U22" t="s">
         <v>30</v>
       </c>
@@ -4696,10 +4699,10 @@
       </c>
     </row>
     <row r="23" spans="17:23">
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
       <c r="U23" t="s">
         <v>31</v>
       </c>
@@ -4711,10 +4714,10 @@
       </c>
     </row>
     <row r="24" spans="17:23">
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
       <c r="U24" t="s">
         <v>32</v>
       </c>
@@ -4726,10 +4729,10 @@
       </c>
     </row>
     <row r="25" spans="17:23">
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
       <c r="U25" t="s">
         <v>33</v>
       </c>
@@ -4741,16 +4744,16 @@
       </c>
     </row>
     <row r="26" spans="17:23">
-      <c r="Q26" s="5" t="s">
+      <c r="Q26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="7">
         <v>19</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="7">
         <v>3.42</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="7">
         <v>3.36</v>
       </c>
       <c r="U26" t="s">
@@ -4764,10 +4767,10 @@
       </c>
     </row>
     <row r="27" spans="17:23">
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
       <c r="U27" t="s">
         <v>36</v>
       </c>
@@ -4779,10 +4782,10 @@
       </c>
     </row>
     <row r="28" spans="17:23">
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
       <c r="U28" t="s">
         <v>37</v>
       </c>
@@ -4794,10 +4797,10 @@
       </c>
     </row>
     <row r="29" spans="17:23">
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
       <c r="U29" t="s">
         <v>38</v>
       </c>
@@ -4809,10 +4812,10 @@
       </c>
     </row>
     <row r="30" spans="17:23">
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
       <c r="U30" t="s">
         <v>39</v>
       </c>
@@ -4824,10 +4827,10 @@
       </c>
     </row>
     <row r="31" spans="17:23">
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
       <c r="U31" t="s">
         <v>40</v>
       </c>
@@ -4839,10 +4842,10 @@
       </c>
     </row>
     <row r="32" spans="17:23">
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
       <c r="U32" t="s">
         <v>41</v>
       </c>
@@ -4854,16 +4857,16 @@
       </c>
     </row>
     <row r="33" spans="17:23">
-      <c r="Q33" s="5" t="s">
+      <c r="Q33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="R33" s="5">
+      <c r="R33" s="7">
         <v>14</v>
       </c>
-      <c r="S33" s="5">
+      <c r="S33" s="7">
         <v>2.96</v>
       </c>
-      <c r="T33" s="5">
+      <c r="T33" s="7">
         <v>3.31</v>
       </c>
       <c r="U33" t="s">
@@ -4877,10 +4880,10 @@
       </c>
     </row>
     <row r="34" spans="17:23">
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
       <c r="U34" t="s">
         <v>44</v>
       </c>
@@ -4892,10 +4895,10 @@
       </c>
     </row>
     <row r="35" spans="17:23">
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
       <c r="U35" t="s">
         <v>45</v>
       </c>
@@ -4907,10 +4910,10 @@
       </c>
     </row>
     <row r="36" spans="17:23">
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
       <c r="U36" t="s">
         <v>46</v>
       </c>
@@ -4922,10 +4925,10 @@
       </c>
     </row>
     <row r="37" spans="17:23">
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
       <c r="U37" t="s">
         <v>47</v>
       </c>
@@ -4937,16 +4940,16 @@
       </c>
     </row>
     <row r="38" spans="17:23">
-      <c r="Q38" s="5" t="s">
+      <c r="Q38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="R38" s="5">
+      <c r="R38" s="7">
         <v>17</v>
       </c>
-      <c r="S38" s="5">
+      <c r="S38" s="7">
         <v>3.47</v>
       </c>
-      <c r="T38" s="5">
+      <c r="T38" s="7">
         <v>3.33</v>
       </c>
       <c r="U38" t="s">
@@ -4960,10 +4963,10 @@
       </c>
     </row>
     <row r="39" spans="17:23">
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
       <c r="U39" t="s">
         <v>50</v>
       </c>
@@ -4975,10 +4978,10 @@
       </c>
     </row>
     <row r="40" spans="17:23">
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
       <c r="U40" t="s">
         <v>51</v>
       </c>
@@ -4990,10 +4993,10 @@
       </c>
     </row>
     <row r="41" spans="17:23">
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
       <c r="U41" t="s">
         <v>52</v>
       </c>
@@ -5005,10 +5008,10 @@
       </c>
     </row>
     <row r="42" spans="17:23">
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
       <c r="U42" t="s">
         <v>47</v>
       </c>
@@ -5020,10 +5023,10 @@
       </c>
     </row>
     <row r="43" spans="17:23">
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
       <c r="U43" t="s">
         <v>53</v>
       </c>
@@ -5035,16 +5038,16 @@
       </c>
     </row>
     <row r="44" spans="17:23">
-      <c r="Q44" s="5" t="s">
+      <c r="Q44" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R44" s="5">
-        <v>9</v>
-      </c>
-      <c r="S44" s="5">
+      <c r="R44" s="7">
+        <v>9</v>
+      </c>
+      <c r="S44" s="7">
         <v>3.5</v>
       </c>
-      <c r="T44" s="5">
+      <c r="T44" s="7">
         <v>3.34</v>
       </c>
       <c r="U44" t="s">
@@ -5058,10 +5061,10 @@
       </c>
     </row>
     <row r="45" spans="17:23">
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
       <c r="U45" t="s">
         <v>56</v>
       </c>
@@ -5073,10 +5076,10 @@
       </c>
     </row>
     <row r="46" spans="17:23">
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
       <c r="U46" t="s">
         <v>57</v>
       </c>

</xml_diff>